<commit_message>
Bugfix size and name
</commit_message>
<xml_diff>
--- a/hardware/doc/PiezoPiano_v13_BOM_20220125_2147.xlsx
+++ b/hardware/doc/PiezoPiano_v13_BOM_20220125_2147.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zapfl\Git\PiezoPiano\hardware\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5D9A392-9847-4229-9EF8-AB7094A67DDC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4320E91-9778-4AB8-9B8E-D904F163E582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18816" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="18696" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -97,9 +97,6 @@
     <t>D1, D4, D6, D7, D8, D9, D10, D11, D12, D13</t>
   </si>
   <si>
-    <t>LED_YELLOW</t>
-  </si>
-  <si>
     <t>8</t>
   </si>
   <si>
@@ -302,6 +299,9 @@
   </si>
   <si>
     <t>Microchip Inc.</t>
+  </si>
+  <si>
+    <t>LED_YELLOW 0603</t>
   </si>
 </sst>
 </file>
@@ -706,7 +706,7 @@
   <dimension ref="A1:G25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -721,42 +721,42 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -853,7 +853,7 @@
         <v>24</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>25</v>
+        <v>93</v>
       </c>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>
@@ -863,16 +863,16 @@
         <v>13</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>12</v>
@@ -880,76 +880,76 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>39</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>46</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,19 +957,19 @@
         <v>7</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="E17" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="E17" s="2" t="s">
+      <c r="F17" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -977,16 +977,16 @@
         <v>13</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>12</v>
@@ -994,135 +994,135 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="D20" s="2" t="s">
+      <c r="E20" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C21" s="2" t="s">
+      <c r="D21" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="E21" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="F21" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B23" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C23" s="2" t="s">
+      <c r="D23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="E23" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="2" t="s">
+      <c r="F23" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="2" t="s">
+      <c r="F24" s="2" t="s">
         <v>33</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>76</v>
-      </c>
-      <c r="B25" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F25" s="2"/>
     </row>

</xml_diff>